<commit_message>
Update microstate list files to remove replicate microstates (v1.4.1).
</commit_message>
<xml_diff>
--- a/physical_properties/pKa/microstates/SM10_microstate_IDs_with_2D_depiction.xlsx
+++ b/physical_properties/pKa/microstates/SM10_microstate_IDs_with_2D_depiction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Microstate List</t>
   </si>
@@ -176,12 +176,6 @@
   </si>
   <si>
     <t>c1ccc(cc1)C(=O)NCC(=O)Nc2[nH+]c3ccccc3s2</t>
-  </si>
-  <si>
-    <t>SM10_micro029</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)C(=O)N/C=C(\Nc2nc3ccccc3s2)/O</t>
   </si>
   <si>
     <t>SM10_micro030</t>
@@ -1492,44 +1486,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="95535750"/>
-          <a:ext cx="3175163" cy="3175163"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>3175163</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>3338</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Picture 32" descr="tmp33.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="98707575"/>
           <a:ext cx="3175163" cy="3175163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1827,7 +1783,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2102,14 +2058,6 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="2:3" s="3" customFormat="1" ht="250.0" customHeight="1">
-      <c r="B34" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Add new microstate to SM10 (v1.5.1).
</commit_message>
<xml_diff>
--- a/physical_properties/pKa/microstates/SM10_microstate_IDs_with_2D_depiction.xlsx
+++ b/physical_properties/pKa/microstates/SM10_microstate_IDs_with_2D_depiction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
   <si>
     <t>Microstate List</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>c1ccc(cc1)C(=O)NCC(=O)Nc2nc3ccccc3s2</t>
+  </si>
+  <si>
+    <t>SM10_micro037</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)C(=O)[N-]CC(=O)Nc2[nH+]c3ccccc3s2</t>
   </si>
 </sst>
 </file>
@@ -1558,6 +1564,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="95535750"/>
+          <a:ext cx="3175163" cy="3175163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3175163</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>3338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32" descr="tmp33.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="98707575"/>
           <a:ext cx="3175163" cy="3175163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1855,7 +1899,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2227,6 +2271,17 @@
         <v>89</v>
       </c>
     </row>
+    <row r="34" spans="2:4" s="3" customFormat="1" ht="250.0" customHeight="1">
+      <c r="B34" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
New microstate ID added fo SM10 (v1.8).
</commit_message>
<xml_diff>
--- a/physical_properties/pKa/microstates/SM10_microstate_IDs_with_2D_depiction.xlsx
+++ b/physical_properties/pKa/microstates/SM10_microstate_IDs_with_2D_depiction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
   <si>
     <t>Microstate List</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>c1ccc(cc1)C(=O)[N-]CC(=O)Nc2[nH+]c3ccccc3s2</t>
+  </si>
+  <si>
+    <t>SM10_micro038</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)C(=O)[NH2+]CC(=O)Nc2[nH+]c3ccccc3s2</t>
   </si>
 </sst>
 </file>
@@ -1602,6 +1608,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="98707575"/>
+          <a:ext cx="3175163" cy="3175163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3175163</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>3338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33" descr="tmp34.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="101879400"/>
           <a:ext cx="3175163" cy="3175163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1899,7 +1943,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2282,6 +2326,17 @@
         <v>91</v>
       </c>
     </row>
+    <row r="35" spans="2:4" s="2" customFormat="1" ht="250.0" customHeight="1">
+      <c r="B35" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>